<commit_message>
excluding lactic acid outliers from analysis
</commit_message>
<xml_diff>
--- a/summary_baseline.xlsx
+++ b/summary_baseline.xlsx
@@ -691,10 +691,10 @@
         <v>-1.594675566921566</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.4474565608894246</v>
+        <v>0.4474565608894246</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.3812195707296989</v>
+        <v>0.3812195707296989</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -777,10 +777,10 @@
         <v>-13.19121830018599</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.05515900976824201</v>
+        <v>0.05515900976824201</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.04665339070962589</v>
+        <v>0.04665339070962589</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>

</xml_diff>